<commit_message>
fix sheet ordereding for all sheets
</commit_message>
<xml_diff>
--- a/testdata/testfile.xlsx
+++ b/testdata/testfile.xlsx
@@ -1,22 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dave/code/github.com/dkoston/xlsx2csv/testdata/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C92CD81-5A08-514E-9D06-639380BBB8FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="13995" windowHeight="5130"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="24700" windowHeight="22680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Foo</t>
   </si>
@@ -28,13 +45,37 @@
   </si>
   <si>
     <t>Quuk</t>
+  </si>
+  <si>
+    <t>column1</t>
+  </si>
+  <si>
+    <t>column2</t>
+  </si>
+  <si>
+    <t>data1</t>
+  </si>
+  <si>
+    <t>data2</t>
+  </si>
+  <si>
+    <t>this</t>
+  </si>
+  <si>
+    <t>thing</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>legit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,17 +108,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -115,9 +164,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -149,9 +198,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -183,9 +250,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -358,16 +443,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -375,7 +460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -389,25 +474,61 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>